<commit_message>
removing mislabelled wildtype strains from perturbed samples
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_1476.xlsx
+++ b/bioSample/bioSample_1476.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">replicate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marker_1</t>
   </si>
   <si>
     <t xml:space="preserve">12.11.14</t>
@@ -82,6 +85,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -163,10 +167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -174,8 +178,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.38"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
@@ -209,28 +213,31 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>90</v>
@@ -241,25 +248,25 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>90</v>
@@ -270,25 +277,25 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>90</v>
@@ -299,25 +306,22 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>90</v>
@@ -328,25 +332,22 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>90</v>
@@ -357,25 +358,22 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>90</v>

</xml_diff>